<commit_message>
expedia and mfd updated
</commit_message>
<xml_diff>
--- a/mfd/Inventario de Materiales Equipos Vehiculos Piloto.xlsx
+++ b/mfd/Inventario de Materiales Equipos Vehiculos Piloto.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/darkesthj/Dev/workspace/mfd/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8AEC5FF-38AD-0144-ABBA-1086C28E9C9B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F0F2511-BDE0-A743-B584-442C1D1E96FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-30240" yWindow="5620" windowWidth="30240" windowHeight="18960" activeTab="1" xr2:uid="{8A56221C-3D16-47BD-B3FF-76CF57FF92C8}"/>
+    <workbookView xWindow="0" yWindow="600" windowWidth="25600" windowHeight="26860" activeTab="1" xr2:uid="{8A56221C-3D16-47BD-B3FF-76CF57FF92C8}"/>
   </bookViews>
   <sheets>
     <sheet name="De Hoja" sheetId="2" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="395" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="330" uniqueCount="80">
   <si>
     <t>Alicate de corte</t>
   </si>
@@ -267,7 +267,16 @@
     <t>Active</t>
   </si>
   <si>
-    <t>Peru</t>
+    <t>ExpectedQuantity</t>
+  </si>
+  <si>
+    <t>ItemCategory</t>
+  </si>
+  <si>
+    <t>Herramienta</t>
+  </si>
+  <si>
+    <t>Consumible</t>
   </si>
 </sst>
 </file>
@@ -305,7 +314,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -337,29 +346,15 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color theme="4" tint="0.39997558519241921"/>
-      </right>
-      <top style="thin">
-        <color theme="4" tint="0.39997558519241921"/>
-      </top>
-      <bottom style="thin">
-        <color theme="4" tint="0.39997558519241921"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1645,16 +1640,15 @@
   <dimension ref="A1:E66"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="181" zoomScaleNormal="181" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.33203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="30.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.83203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="25.83203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="25.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="28.1640625" customWidth="1"/>
+    <col min="4" max="4" width="6" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
@@ -1662,16 +1656,16 @@
         <v>53</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>54</v>
+        <v>76</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>44</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="E1" s="4" t="s">
         <v>75</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>77</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
@@ -1684,11 +1678,11 @@
       <c r="C2" t="s">
         <v>74</v>
       </c>
-      <c r="D2" t="s">
-        <v>76</v>
+      <c r="D2" t="b">
+        <v>1</v>
       </c>
       <c r="E2" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
@@ -1701,11 +1695,11 @@
       <c r="C3" t="s">
         <v>74</v>
       </c>
-      <c r="D3" t="s">
-        <v>76</v>
+      <c r="D3" t="b">
+        <v>1</v>
       </c>
       <c r="E3" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
@@ -1718,11 +1712,11 @@
       <c r="C4" t="s">
         <v>74</v>
       </c>
-      <c r="D4" t="s">
-        <v>76</v>
+      <c r="D4" t="b">
+        <v>1</v>
       </c>
       <c r="E4" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
@@ -1735,11 +1729,11 @@
       <c r="C5" t="s">
         <v>74</v>
       </c>
-      <c r="D5" t="s">
-        <v>76</v>
+      <c r="D5" t="b">
+        <v>1</v>
       </c>
       <c r="E5" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
@@ -1752,11 +1746,11 @@
       <c r="C6" t="s">
         <v>74</v>
       </c>
-      <c r="D6" t="s">
-        <v>76</v>
+      <c r="D6" t="b">
+        <v>1</v>
       </c>
       <c r="E6" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
@@ -1769,11 +1763,11 @@
       <c r="C7" t="s">
         <v>74</v>
       </c>
-      <c r="D7" t="s">
-        <v>76</v>
+      <c r="D7" t="b">
+        <v>1</v>
       </c>
       <c r="E7" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
@@ -1786,11 +1780,11 @@
       <c r="C8" t="s">
         <v>74</v>
       </c>
-      <c r="D8" t="s">
-        <v>76</v>
+      <c r="D8" t="b">
+        <v>1</v>
       </c>
       <c r="E8" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
@@ -1803,11 +1797,11 @@
       <c r="C9" t="s">
         <v>74</v>
       </c>
-      <c r="D9" t="s">
-        <v>76</v>
+      <c r="D9" t="b">
+        <v>1</v>
       </c>
       <c r="E9" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
@@ -1820,11 +1814,11 @@
       <c r="C10" t="s">
         <v>74</v>
       </c>
-      <c r="D10" t="s">
-        <v>76</v>
+      <c r="D10" t="b">
+        <v>1</v>
       </c>
       <c r="E10" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
@@ -1837,11 +1831,11 @@
       <c r="C11" t="s">
         <v>74</v>
       </c>
-      <c r="D11" t="s">
-        <v>76</v>
+      <c r="D11" t="b">
+        <v>1</v>
       </c>
       <c r="E11" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
@@ -1854,11 +1848,11 @@
       <c r="C12" t="s">
         <v>74</v>
       </c>
-      <c r="D12" t="s">
-        <v>76</v>
+      <c r="D12" t="b">
+        <v>1</v>
       </c>
       <c r="E12" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
@@ -1871,11 +1865,11 @@
       <c r="C13" t="s">
         <v>74</v>
       </c>
-      <c r="D13" t="s">
-        <v>76</v>
+      <c r="D13" t="b">
+        <v>1</v>
       </c>
       <c r="E13" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
@@ -1888,11 +1882,11 @@
       <c r="C14" t="s">
         <v>74</v>
       </c>
-      <c r="D14" t="s">
-        <v>76</v>
+      <c r="D14" t="b">
+        <v>1</v>
       </c>
       <c r="E14" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
@@ -1905,11 +1899,11 @@
       <c r="C15" t="s">
         <v>74</v>
       </c>
-      <c r="D15" t="s">
-        <v>76</v>
+      <c r="D15" t="b">
+        <v>1</v>
       </c>
       <c r="E15" t="s">
-        <v>74</v>
+        <v>79</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
@@ -1922,11 +1916,11 @@
       <c r="C16" t="s">
         <v>74</v>
       </c>
-      <c r="D16" t="s">
-        <v>76</v>
+      <c r="D16" t="b">
+        <v>1</v>
       </c>
       <c r="E16" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.2">
@@ -1939,11 +1933,11 @@
       <c r="C17" t="s">
         <v>74</v>
       </c>
-      <c r="D17" t="s">
-        <v>76</v>
+      <c r="D17" t="b">
+        <v>1</v>
       </c>
       <c r="E17" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.2">
@@ -1956,11 +1950,11 @@
       <c r="C18" t="s">
         <v>74</v>
       </c>
-      <c r="D18" t="s">
-        <v>76</v>
+      <c r="D18" t="b">
+        <v>1</v>
       </c>
       <c r="E18" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.2">
@@ -1973,11 +1967,11 @@
       <c r="C19" t="s">
         <v>74</v>
       </c>
-      <c r="D19" t="s">
-        <v>76</v>
+      <c r="D19" t="b">
+        <v>1</v>
       </c>
       <c r="E19" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.2">
@@ -1990,11 +1984,11 @@
       <c r="C20" t="s">
         <v>74</v>
       </c>
-      <c r="D20" t="s">
-        <v>76</v>
+      <c r="D20" t="b">
+        <v>1</v>
       </c>
       <c r="E20" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.2">
@@ -2007,11 +2001,11 @@
       <c r="C21" t="s">
         <v>74</v>
       </c>
-      <c r="D21" t="s">
-        <v>76</v>
+      <c r="D21" t="b">
+        <v>1</v>
       </c>
       <c r="E21" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.2">
@@ -2024,11 +2018,11 @@
       <c r="C22" t="s">
         <v>74</v>
       </c>
-      <c r="D22" t="s">
-        <v>76</v>
+      <c r="D22" t="b">
+        <v>1</v>
       </c>
       <c r="E22" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.2">
@@ -2041,11 +2035,11 @@
       <c r="C23" t="s">
         <v>74</v>
       </c>
-      <c r="D23" t="s">
-        <v>76</v>
+      <c r="D23" t="b">
+        <v>1</v>
       </c>
       <c r="E23" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.2">
@@ -2058,11 +2052,11 @@
       <c r="C24" t="s">
         <v>74</v>
       </c>
-      <c r="D24" t="s">
-        <v>76</v>
+      <c r="D24" t="b">
+        <v>1</v>
       </c>
       <c r="E24" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.2">
@@ -2075,11 +2069,11 @@
       <c r="C25" t="s">
         <v>74</v>
       </c>
-      <c r="D25" t="s">
-        <v>76</v>
+      <c r="D25" t="b">
+        <v>1</v>
       </c>
       <c r="E25" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.2">
@@ -2092,11 +2086,11 @@
       <c r="C26" t="s">
         <v>74</v>
       </c>
-      <c r="D26" t="s">
-        <v>76</v>
+      <c r="D26" t="b">
+        <v>1</v>
       </c>
       <c r="E26" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.2">
@@ -2109,11 +2103,11 @@
       <c r="C27" t="s">
         <v>74</v>
       </c>
-      <c r="D27" t="s">
-        <v>76</v>
+      <c r="D27" t="b">
+        <v>1</v>
       </c>
       <c r="E27" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.2">
@@ -2126,11 +2120,11 @@
       <c r="C28" t="s">
         <v>74</v>
       </c>
-      <c r="D28" t="s">
-        <v>76</v>
+      <c r="D28" t="b">
+        <v>1</v>
       </c>
       <c r="E28" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.2">
@@ -2143,11 +2137,11 @@
       <c r="C29" t="s">
         <v>74</v>
       </c>
-      <c r="D29" t="s">
-        <v>76</v>
+      <c r="D29" t="b">
+        <v>1</v>
       </c>
       <c r="E29" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.2">
@@ -2160,11 +2154,11 @@
       <c r="C30" t="s">
         <v>74</v>
       </c>
-      <c r="D30" t="s">
-        <v>76</v>
+      <c r="D30" t="b">
+        <v>1</v>
       </c>
       <c r="E30" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.2">
@@ -2177,11 +2171,11 @@
       <c r="C31" t="s">
         <v>74</v>
       </c>
-      <c r="D31" t="s">
-        <v>76</v>
+      <c r="D31" t="b">
+        <v>1</v>
       </c>
       <c r="E31" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.2">
@@ -2194,11 +2188,11 @@
       <c r="C32" t="s">
         <v>74</v>
       </c>
-      <c r="D32" t="s">
-        <v>76</v>
+      <c r="D32" t="b">
+        <v>1</v>
       </c>
       <c r="E32" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.2">
@@ -2211,11 +2205,11 @@
       <c r="C33" t="s">
         <v>74</v>
       </c>
-      <c r="D33" t="s">
-        <v>76</v>
+      <c r="D33" t="b">
+        <v>1</v>
       </c>
       <c r="E33" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.2">
@@ -2228,11 +2222,11 @@
       <c r="C34" t="s">
         <v>74</v>
       </c>
-      <c r="D34" t="s">
-        <v>76</v>
+      <c r="D34" t="b">
+        <v>1</v>
       </c>
       <c r="E34" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.2">
@@ -2245,11 +2239,11 @@
       <c r="C35" t="s">
         <v>74</v>
       </c>
-      <c r="D35" t="s">
-        <v>76</v>
+      <c r="D35" t="b">
+        <v>1</v>
       </c>
       <c r="E35" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.2">
@@ -2262,11 +2256,11 @@
       <c r="C36" t="s">
         <v>74</v>
       </c>
-      <c r="D36" t="s">
-        <v>76</v>
+      <c r="D36" t="b">
+        <v>1</v>
       </c>
       <c r="E36" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.2">
@@ -2279,11 +2273,11 @@
       <c r="C37" t="s">
         <v>74</v>
       </c>
-      <c r="D37" t="s">
-        <v>76</v>
+      <c r="D37" t="b">
+        <v>1</v>
       </c>
       <c r="E37" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.2">
@@ -2296,11 +2290,11 @@
       <c r="C38" t="s">
         <v>74</v>
       </c>
-      <c r="D38" t="s">
-        <v>76</v>
+      <c r="D38" t="b">
+        <v>1</v>
       </c>
       <c r="E38" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.2">
@@ -2313,11 +2307,11 @@
       <c r="C39" t="s">
         <v>74</v>
       </c>
-      <c r="D39" t="s">
-        <v>76</v>
+      <c r="D39" t="b">
+        <v>1</v>
       </c>
       <c r="E39" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.2">
@@ -2330,11 +2324,11 @@
       <c r="C40" t="s">
         <v>74</v>
       </c>
-      <c r="D40" t="s">
-        <v>76</v>
+      <c r="D40" t="b">
+        <v>1</v>
       </c>
       <c r="E40" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.2">
@@ -2347,11 +2341,11 @@
       <c r="C41" t="s">
         <v>74</v>
       </c>
-      <c r="D41" t="s">
-        <v>76</v>
+      <c r="D41" t="b">
+        <v>1</v>
       </c>
       <c r="E41" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.2">
@@ -2364,11 +2358,11 @@
       <c r="C42" t="s">
         <v>74</v>
       </c>
-      <c r="D42" t="s">
-        <v>76</v>
+      <c r="D42" t="b">
+        <v>1</v>
       </c>
       <c r="E42" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.2">
@@ -2381,11 +2375,11 @@
       <c r="C43" t="s">
         <v>74</v>
       </c>
-      <c r="D43" t="s">
-        <v>76</v>
+      <c r="D43" t="b">
+        <v>1</v>
       </c>
       <c r="E43" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.2">
@@ -2398,11 +2392,11 @@
       <c r="C44" t="s">
         <v>74</v>
       </c>
-      <c r="D44" t="s">
-        <v>76</v>
+      <c r="D44" t="b">
+        <v>1</v>
       </c>
       <c r="E44" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.2">
@@ -2415,11 +2409,11 @@
       <c r="C45" t="s">
         <v>74</v>
       </c>
-      <c r="D45" t="s">
-        <v>76</v>
+      <c r="D45" t="b">
+        <v>1</v>
       </c>
       <c r="E45" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.2">
@@ -2432,11 +2426,11 @@
       <c r="C46" t="s">
         <v>74</v>
       </c>
-      <c r="D46" t="s">
-        <v>76</v>
+      <c r="D46" t="b">
+        <v>1</v>
       </c>
       <c r="E46" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.2">
@@ -2449,11 +2443,11 @@
       <c r="C47" t="s">
         <v>74</v>
       </c>
-      <c r="D47" t="s">
-        <v>76</v>
+      <c r="D47" t="b">
+        <v>1</v>
       </c>
       <c r="E47" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.2">
@@ -2466,11 +2460,11 @@
       <c r="C48" t="s">
         <v>74</v>
       </c>
-      <c r="D48" t="s">
-        <v>76</v>
+      <c r="D48" t="b">
+        <v>1</v>
       </c>
       <c r="E48" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.2">
@@ -2483,11 +2477,11 @@
       <c r="C49" t="s">
         <v>74</v>
       </c>
-      <c r="D49" t="s">
-        <v>76</v>
+      <c r="D49" t="b">
+        <v>1</v>
       </c>
       <c r="E49" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.2">
@@ -2500,11 +2494,11 @@
       <c r="C50" t="s">
         <v>74</v>
       </c>
-      <c r="D50" t="s">
-        <v>76</v>
+      <c r="D50" t="b">
+        <v>1</v>
       </c>
       <c r="E50" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.2">
@@ -2517,11 +2511,11 @@
       <c r="C51" t="s">
         <v>74</v>
       </c>
-      <c r="D51" t="s">
-        <v>76</v>
+      <c r="D51" t="b">
+        <v>1</v>
       </c>
       <c r="E51" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.2">
@@ -2534,11 +2528,11 @@
       <c r="C52" t="s">
         <v>74</v>
       </c>
-      <c r="D52" t="s">
-        <v>76</v>
+      <c r="D52" t="b">
+        <v>1</v>
       </c>
       <c r="E52" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.2">
@@ -2551,11 +2545,11 @@
       <c r="C53" t="s">
         <v>74</v>
       </c>
-      <c r="D53" t="s">
-        <v>76</v>
+      <c r="D53" t="b">
+        <v>1</v>
       </c>
       <c r="E53" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.2">
@@ -2568,11 +2562,11 @@
       <c r="C54" t="s">
         <v>74</v>
       </c>
-      <c r="D54" t="s">
-        <v>76</v>
+      <c r="D54" t="b">
+        <v>1</v>
       </c>
       <c r="E54" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.2">
@@ -2585,11 +2579,11 @@
       <c r="C55" t="s">
         <v>74</v>
       </c>
-      <c r="D55" t="s">
-        <v>76</v>
+      <c r="D55" t="b">
+        <v>1</v>
       </c>
       <c r="E55" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.2">
@@ -2602,11 +2596,11 @@
       <c r="C56" t="s">
         <v>74</v>
       </c>
-      <c r="D56" t="s">
-        <v>76</v>
+      <c r="D56" t="b">
+        <v>1</v>
       </c>
       <c r="E56" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.2">
@@ -2619,11 +2613,11 @@
       <c r="C57" t="s">
         <v>74</v>
       </c>
-      <c r="D57" t="s">
-        <v>76</v>
+      <c r="D57" t="b">
+        <v>1</v>
       </c>
       <c r="E57" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.2">
@@ -2636,11 +2630,11 @@
       <c r="C58" t="s">
         <v>74</v>
       </c>
-      <c r="D58" t="s">
-        <v>76</v>
+      <c r="D58" t="b">
+        <v>1</v>
       </c>
       <c r="E58" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.2">
@@ -2653,11 +2647,11 @@
       <c r="C59" t="s">
         <v>74</v>
       </c>
-      <c r="D59" t="s">
-        <v>76</v>
+      <c r="D59" t="b">
+        <v>1</v>
       </c>
       <c r="E59" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.2">
@@ -2670,11 +2664,11 @@
       <c r="C60" t="s">
         <v>74</v>
       </c>
-      <c r="D60" t="s">
-        <v>76</v>
+      <c r="D60" t="b">
+        <v>1</v>
       </c>
       <c r="E60" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.2">
@@ -2687,11 +2681,11 @@
       <c r="C61" t="s">
         <v>74</v>
       </c>
-      <c r="D61" t="s">
-        <v>76</v>
+      <c r="D61" t="b">
+        <v>1</v>
       </c>
       <c r="E61" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.2">
@@ -2704,11 +2698,11 @@
       <c r="C62" t="s">
         <v>74</v>
       </c>
-      <c r="D62" t="s">
-        <v>76</v>
+      <c r="D62" t="b">
+        <v>1</v>
       </c>
       <c r="E62" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.2">
@@ -2721,11 +2715,11 @@
       <c r="C63" t="s">
         <v>74</v>
       </c>
-      <c r="D63" t="s">
-        <v>76</v>
+      <c r="D63" t="b">
+        <v>1</v>
       </c>
       <c r="E63" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.2">
@@ -2738,11 +2732,11 @@
       <c r="C64" t="s">
         <v>74</v>
       </c>
-      <c r="D64" t="s">
-        <v>76</v>
+      <c r="D64" t="b">
+        <v>1</v>
       </c>
       <c r="E64" t="s">
-        <v>74</v>
+        <v>79</v>
       </c>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.2">
@@ -2755,11 +2749,11 @@
       <c r="C65" t="s">
         <v>74</v>
       </c>
-      <c r="D65" t="s">
-        <v>76</v>
+      <c r="D65" t="b">
+        <v>1</v>
       </c>
       <c r="E65" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.2">
@@ -2772,11 +2766,11 @@
       <c r="C66" t="s">
         <v>74</v>
       </c>
-      <c r="D66" t="s">
-        <v>76</v>
+      <c r="D66" t="b">
+        <v>1</v>
       </c>
       <c r="E66" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
     </row>
   </sheetData>

</xml_diff>